<commit_message>
20180626 updated focus on python file operation
</commit_message>
<xml_diff>
--- a/dailyworkRecord.xlsx
+++ b/dailyworkRecord.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="49">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,14 @@
   </si>
   <si>
     <t>learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python edit file//test case auto check …interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>review</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,6 +376,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -700,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G131"/>
+  <dimension ref="B1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1442,7 +1453,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="8"/>
-      <c r="E67" s="25" t="s">
+      <c r="E67" s="26" t="s">
         <v>35</v>
       </c>
       <c r="F67" s="14"/>
@@ -1454,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="D68" s="8"/>
-      <c r="E68" s="25"/>
+      <c r="E68" s="26"/>
       <c r="F68" s="15"/>
       <c r="G68" s="9"/>
     </row>
@@ -1464,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="D69" s="8"/>
-      <c r="E69" s="25"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="14"/>
       <c r="G69" s="9"/>
     </row>
@@ -1474,7 +1485,7 @@
         <v>11</v>
       </c>
       <c r="D70" s="8"/>
-      <c r="E70" s="25"/>
+      <c r="E70" s="26"/>
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
     </row>
@@ -1511,7 +1522,7 @@
         <v>8</v>
       </c>
       <c r="D74" s="8"/>
-      <c r="E74" s="25" t="s">
+      <c r="E74" s="26" t="s">
         <v>36</v>
       </c>
       <c r="F74" s="17"/>
@@ -1523,7 +1534,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="8"/>
-      <c r="E75" s="25"/>
+      <c r="E75" s="26"/>
       <c r="F75" s="15"/>
       <c r="G75" s="9"/>
     </row>
@@ -1533,7 +1544,7 @@
         <v>10</v>
       </c>
       <c r="D76" s="8"/>
-      <c r="E76" s="25"/>
+      <c r="E76" s="26"/>
       <c r="F76" s="17"/>
       <c r="G76" s="9"/>
     </row>
@@ -1543,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="D77" s="8"/>
-      <c r="E77" s="25"/>
+      <c r="E77" s="26"/>
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
     </row>
@@ -1588,7 +1599,7 @@
         <v>8</v>
       </c>
       <c r="D83" s="8"/>
-      <c r="E83" s="25" t="s">
+      <c r="E83" s="26" t="s">
         <v>38</v>
       </c>
       <c r="F83" s="18"/>
@@ -1600,7 +1611,7 @@
         <v>9</v>
       </c>
       <c r="D84" s="8"/>
-      <c r="E84" s="25"/>
+      <c r="E84" s="26"/>
       <c r="F84" s="15"/>
       <c r="G84" s="9"/>
     </row>
@@ -1610,7 +1621,7 @@
         <v>10</v>
       </c>
       <c r="D85" s="8"/>
-      <c r="E85" s="25"/>
+      <c r="E85" s="26"/>
       <c r="F85" s="18"/>
       <c r="G85" s="9"/>
     </row>
@@ -1620,7 +1631,7 @@
         <v>11</v>
       </c>
       <c r="D86" s="8"/>
-      <c r="E86" s="25"/>
+      <c r="E86" s="26"/>
       <c r="F86" s="8"/>
       <c r="G86" s="9"/>
     </row>
@@ -2081,6 +2092,81 @@
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
       <c r="G131" s="13"/>
+    </row>
+    <row r="133" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B134" s="2">
+        <v>43277</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G134" s="5"/>
+    </row>
+    <row r="135" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="B135" s="6"/>
+      <c r="C135" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" s="8"/>
+      <c r="E135" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F135" s="25"/>
+      <c r="G135" s="9"/>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B136" s="6"/>
+      <c r="C136" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" s="8"/>
+      <c r="E136" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F136" s="15"/>
+      <c r="G136" s="9"/>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B137" s="6"/>
+      <c r="C137" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" s="8"/>
+      <c r="E137" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F137" s="25"/>
+      <c r="G137" s="9"/>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B138" s="6"/>
+      <c r="C138" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F138" s="8"/>
+      <c r="G138" s="9"/>
+    </row>
+    <row r="139" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="10"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>